<commit_message>
Adding additional descriptions of scenes
</commit_message>
<xml_diff>
--- a/shot_scene/scene_description_test.xlsx
+++ b/shot_scene/scene_description_test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="237">
   <si>
     <t>AnotherMissOh16_019_0000</t>
   </si>
@@ -215,584 +215,650 @@
     <t>AnotherMissOh17_054_0000</t>
   </si>
   <si>
+    <t>AnotherMissOh17_057_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_001_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_002_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_003_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_004_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_005_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_006_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_007_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_008_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_009_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_010_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_011_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_012_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_013_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_014_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_015_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_016_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_017_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_018_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_019_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_020_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_021_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_022_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_023_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_024_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_025_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_026_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_027_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_028_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_029_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_030_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_031_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_032_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_033_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_034_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_035_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_036_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_037_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_038_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_039_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_040_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_041_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_042_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_043_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_044_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_045_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_046_0000</t>
+  </si>
+  <si>
+    <t>AnotherMissOh18_047_0000</t>
+  </si>
+  <si>
+    <t>Additional description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh16_001_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh16_002_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh16_003_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh16_004_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh16_005_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh16_006_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh16_007_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh16_008_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh16_009_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh16_010_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh16_011_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh16_012_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh16_013_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh16_014_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh16_015_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh16_016_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh16_017_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh16_018_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung1 is sad to see Dokyung's face bruised.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung1 surprises Dokyung while Dokyung is leaving the house to give Haeyoung1 a ride to work.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jinsang, Hun, Sukyung talk about Jinsang and Sukyung's kiss last night.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Soontack, Dokyung, and person(doctor) talk about Dokyung's future predictions.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung buy flowers and visits Haeyoung1's company.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung1 is happy to see the flowers that Dokyung left at Haeyoung1's seat.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taejin's partner and Chairman talk about what Taejin's parnter did.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung1 returns home and prepares ingredients to make food</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deogi monologues about her feelings toward Haeyoung1 while coming home from buying burdock at a market</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jinsang talk on phone with Hun about discomfort with Sukyung</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anna and Hun meet Heeran in office and Anna and Heeran talk about Hun.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sukyung look at Jinsang smoking a cigarette and reminisces about old memories.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taejin and Taejin's partner drink and talk about revenge against Dokyung.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung and Haeyoung1 talk about the flower that Dokyung bought for Haeyoung1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung and Haeyoung1 talk about the flowers while they brush teeths in bathroom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung asks Haeyoung1 why she fall in love with me at first sight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sangseok, Yijoon, Gitae, and Hun are angry and surprised by the seizure sticker.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hun, Sangseok, Yijoon, Gitae think that Jiya is the reason for the seizure sticker.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jiya visits a man and learns why the seizure sticker was posted in office.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taejin and Chairman talk about seizure of Dokyung's property.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung and Haeyoung1 are on a date when Dokyung receives a phone call from Jinsang.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anna and Hun create and record sound for a video.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jinsang realize that Taejin has seized Dokyung's property and discusses with Dokyung.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung1 and Haeyoung2 have a lunch together and talk about their feelings for each other.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jiya appears and takes her anger on Haeyoung2 who is walking with Haeyoung1, and Haeyoung1 tries to stop her.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung1 explains to Jiya about the relationship with Dokyung at the café, and Jitta scolds Haeyoung1 to break up Dokyung</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung2 argues with Jiya coming out of the café</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung drinks at a restaurant with Hun, Gitae, Yijoon, and Sangseok and briefly talks about the current situation at the company</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taejin is dumbfounded when he sees Dokyung smiling at the restaurant, so he deliberately goes into the restaurant and pays for Dokyung.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sukyung tells Jinsang about her decision regarding relationship with Jinsang and tells Jinsang to leave house.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sukyung goes out with Jinsang to see him off from home. Jinsang shed tears feeling sorry for Sukyung while walking.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh16_032_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung1 comes to Taejin's house and asks Taejin to talk outside, but Taejin ignores and goes into room.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung1 opens her heart to Taejin about her feelings of being dumped the day before the wedding. Haeyoung1 talks about Dokyung to Taejin and leave</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh16_034_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sangseok, Yijoon, Gitae, and Hun are sad to be separated from Dokyung, so they cry and drink soju. Dokyung leaves.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh17_001_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung waits Haeyoung1 in front of company with an umbrella for Haeyoung1, and meets Haeyoung1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung1 scolds Dokyung for bringing two umbrellas. Afterwards, Do-kyung walks away sharing Haeyoung1's umbrella, and Dokyung tells Haeyoung1 that he loves her.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung1 scolds Dokyung for bringing two umbrellas. Afterwards, Do-kyung walks away sharing Haeyoung1's umbrella, and Dokyung tells Haeyoung1 that he loves her.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh16_036_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh17_002_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung1 shouts out the window to Dokyung that she loves Dokyung on the bus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deogi and Kyungsu in the front yard and surprised to see Haeyoung1 and Dokyung at the door.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh17_004_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deogi and Kyungsu come into the house and disapprove of Haeyoung1, who likes Dokyung.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung looks out the window on a bus on the way home and is thankful.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung1 wakes up, looks in the mirror and is happy because Haeyoung1 is loved.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung1 is happy even though Haeyoung1 misses the bus.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung wakes up Jinsang who is sleeping in his office, and tries to take him sauna.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jinsang confesses his feelings to Dokyung and receives comfort.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh17_010_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sukyung is working out at the office when Sungjin comes to receive approval, and Sukyung rejects.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh17_011_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sangseok and Hun tell Dokyung that they are not leaving, and Jiya enters the room.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jiya persuades Dokyung to seek forgiveness from the Chairman, but Dokyung says it is his fault.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jiya, feeling strange, calls Sukyung and tells him that Dokyung is strange.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung1 is happy looking at flowers and receives a call from Dokyung asking to eat dinner with Sukyung.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung1 and Sukyung meet Dokyung and Hun in front of their house</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung1, Dokyung, Hun, and Sukyung prepare and eat dinner together.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung1 and Dokyung talk about Jinsang and consider what music want to listen, and Dokyung gives Haeyoung1 a gift a bracelet as a gift</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jinsang dances with many women</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hun enters the club while Jinsang is having fun with his friends.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jinsang returns to the table with his friends and drinks beer.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hun spots Jinsang and shouts, so Jinsang goes to catch Hun.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hun and Jinsang fight on the street</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jinsang returns to the club to have fun again, but leaves the club after seeing Melon at table.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung and Haeyoung1 greet each other in front of Haeyoung1’s house</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung finds Taejin on the pedestrian overpass and saves Taejin from falling.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung sees Taejin drunk and passes by, but then goes back to Taejin.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung2 asks the Chairman for a favor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung2 and Taejin meet and talk in front of the Chairman's house</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jinsang goes to Sukyung's company and keeps trying to talk, but Sukyung ignores him.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jinsang blocks the elevator door from closing and tells Sukyung to kiss him.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sungjin and the company are watching Jinsang and Sukyung kiss passionately</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung1 meets Haeyoung2 and thanks each other.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AnotherMissOh17_033_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung is suffering while seeing an illusion.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung is traveling in a car and is worried because he keeps seeing visions.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Soontack suggests to the doctor that he should hypnotize Dokyung.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung is under hypnosis, and the situation is explained by Dokyung</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung is driving and Haeyoung1 is meditating</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung1 is meditating</t>
+  </si>
+  <si>
+    <t>Dokyung calls Haeyoung1 by text and Haeyoung1 goes to the front of the house.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung and Haeyoung1 talk about when they first saw each other, and Dokyung confides his situation to Haeyoung1.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deogi tells Haeyoung1 to ask Dokyung to come in for breakfast.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung waits leaning against the car in front of Haeyoung1’s house.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deogi, Kyungsu, Haeyoung1, and Dokyung eat breakfast together</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taejin looks at shoes of Taejin's partner while driving and notices that Taejin's partner was at the Chairman's house.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taejin is scammed and his company is searched and seized.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taejin visits the Chairman but does not meet him.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taejin searches for his business partner while driving.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taejin follows his business partner and fights with the partner.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung calls Haeyoung1 and suggests that Dokyung and Haeyoung1 go on a trip.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung1 gradually understands what Dokyung said before.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung confronts Taejin in front of the building.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung1 runs to find Dokyung.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung has a premonition of the future he saw and runs away from Taejin after calling Haeyoung1.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung sees Haeyoung1 coming from the other side and runs to hug him.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>AnotherMissOh17_055_0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Soontack's senior doctor and person are talking.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>AnotherMissOh17_056_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh17_057_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_001_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_002_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_003_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_004_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_005_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_006_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_007_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_008_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_009_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_010_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_011_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_012_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_013_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_014_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_015_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_016_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_017_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_018_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_019_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_020_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_021_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_022_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_023_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_024_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_025_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_026_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_027_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_028_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_029_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_030_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_031_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_032_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_033_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_034_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_035_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_036_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_037_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_038_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_039_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_040_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_041_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_042_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_043_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_044_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_045_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_046_0000</t>
-  </si>
-  <si>
-    <t>AnotherMissOh18_047_0000</t>
-  </si>
-  <si>
-    <t>Additional description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh16_001_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh16_002_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh16_003_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh16_004_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh16_005_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh16_006_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh16_007_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh16_008_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh16_009_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh16_010_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh16_011_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh16_012_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh16_013_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh16_014_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh16_015_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh16_016_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh16_017_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh16_018_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Haeyoung1 is sad to see Dokyung's face bruised.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Haeyoung1 surprises Dokyung while Dokyung is leaving the house to give Haeyoung1 a ride to work.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jinsang, Hun, Sukyung talk about Jinsang and Sukyung's kiss last night.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Soontack, Dokyung, and person(doctor) talk about Dokyung's future predictions.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dokyung buy flowers and visits Haeyoung1's company.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Haeyoung1 is happy to see the flowers that Dokyung left at Haeyoung1's seat.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Taejin's partner and Chairman talk about what Taejin's parnter did.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Haeyoung1 returns home and prepares ingredients to make food</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Deogi monologues about her feelings toward Haeyoung1 while coming home from buying burdock at a market</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jinsang talk on phone with Hun about discomfort with Sukyung</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Anna and Hun meet Heeran in office and Anna and Heeran talk about Hun.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sukyung look at Jinsang smoking a cigarette and reminisces about old memories.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Taejin and Taejin's partner drink and talk about revenge against Dokyung.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dokyung and Haeyoung1 talk about the flower that Dokyung bought for Haeyoung1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dokyung and Haeyoung1 talk about the flowers while they brush teeths in bathroom</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dokyung asks Haeyoung1 why she fall in love with me at first sight</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sangseok, Yijoon, Gitae, and Hun are angry and surprised by the seizure sticker.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hun, Sangseok, Yijoon, Gitae think that Jiya is the reason for the seizure sticker.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jiya visits a man and learns why the seizure sticker was posted in office.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Taejin and Chairman talk about seizure of Dokyung's property.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dokyung and Haeyoung1 are on a date when Dokyung receives a phone call from Jinsang.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Anna and Hun create and record sound for a video.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jinsang realize that Taejin has seized Dokyung's property and discusses with Dokyung.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Haeyoung1 and Haeyoung2 have a lunch together and talk about their feelings for each other.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jiya appears and takes her anger on Haeyoung2 who is walking with Haeyoung1, and Haeyoung1 tries to stop her.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Haeyoung1 explains to Jiya about the relationship with Dokyung at the café, and Jitta scolds Haeyoung1 to break up Dokyung</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Haeyoung2 argues with Jiya coming out of the café</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dokyung drinks at a restaurant with Hun, Gitae, Yijoon, and Sangseok and briefly talks about the current situation at the company</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Taejin is dumbfounded when he sees Dokyung smiling at the restaurant, so he deliberately goes into the restaurant and pays for Dokyung.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sukyung tells Jinsang about her decision regarding relationship with Jinsang and tells Jinsang to leave house.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sukyung goes out with Jinsang to see him off from home. Jinsang shed tears feeling sorry for Sukyung while walking.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh16_032_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Haeyoung1 comes to Taejin's house and asks Taejin to talk outside, but Taejin ignores and goes into room.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Haeyoung1 opens her heart to Taejin about her feelings of being dumped the day before the wedding. Haeyoung1 talks about Dokyung to Taejin and leave</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh16_034_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sangseok, Yijoon, Gitae, and Hun are sad to be separated from Dokyung, so they cry and drink soju. Dokyung leaves.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh17_001_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dokyung waits Haeyoung1 in front of company with an umbrella for Haeyoung1, and meets Haeyoung1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Haeyoung1 scolds Dokyung for bringing two umbrellas. Afterwards, Do-kyung walks away sharing Haeyoung1's umbrella, and Dokyung tells Haeyoung1 that he loves her.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Haeyoung1 scolds Dokyung for bringing two umbrellas. Afterwards, Do-kyung walks away sharing Haeyoung1's umbrella, and Dokyung tells Haeyoung1 that he loves her.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh16_036_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh17_002_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Haeyoung1 shouts out the window to Dokyung that she loves Dokyung on the bus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Deogi and Kyungsu in the front yard and surprised to see Haeyoung1 and Dokyung at the door.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh17_004_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Deogi and Kyungsu come into the house and disapprove of Haeyoung1, who likes Dokyung.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dokyung looks out the window on a bus on the way home and is thankful.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Haeyoung1 wakes up, looks in the mirror and is happy because Haeyoung1 is loved.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Haeyoung1 is happy even though Haeyoung1 misses the bus.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dokyung wakes up Jinsang who is sleeping in his office, and tries to take him sauna.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jinsang confesses his feelings to Dokyung and receives comfort.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh17_010_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sukyung is working out at the office when Sungjin comes to receive approval, and Sukyung rejects.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh17_011_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sangseok and Hun tell Dokyung that they are not leaving, and Jiya enters the room.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jiya persuades Dokyung to seek forgiveness from the Chairman, but Dokyung says it is his fault.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jiya, feeling strange, calls Sukyung and tells him that Dokyung is strange.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Haeyoung1 is happy looking at flowers and receives a call from Dokyung asking to eat dinner with Sukyung.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Haeyoung1 and Sukyung meet Dokyung and Hun in front of their house</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Haeyoung1, Dokyung, Hun, and Sukyung prepare and eat dinner together.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Haeyoung1 and Dokyung talk about Jinsang and consider what music want to listen, and Dokyung gives Haeyoung1 a gift a bracelet as a gift</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jinsang dances with many women</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hun enters the club while Jinsang is having fun with his friends.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jinsang returns to the table with his friends and drinks beer.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hun spots Jinsang and shouts, so Jinsang goes to catch Hun.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hun and Jinsang fight on the street</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jinsang returns to the club to have fun again, but leaves the club after seeing Melon at table.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dokyung and Haeyoung1 greet each other in front of Haeyoung1’s house</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dokyung finds Taejin on the pedestrian overpass and saves Taejin from falling.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dokyung sees Taejin drunk and passes by, but then goes back to Taejin.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Haeyoung2 asks the Chairman for a favor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Haeyoung2 and Taejin meet and talk in front of the Chairman's house</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jinsang goes to Sukyung's company and keeps trying to talk, but Sukyung ignores him.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jinsang blocks the elevator door from closing and tells Sukyung to kiss him.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sungjin and the company are watching Jinsang and Sukyung kiss passionately</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Haeyoung1 meets Haeyoung2 and thanks each other.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AnotherMissOh17_033_0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dokyung is suffering while seeing an illusion.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dokyung is traveling in a car and is worried because he keeps seeing visions.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Soontack suggests to the doctor that he should hypnotize Dokyung.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dokyung is under hypnosis, and the situation is explained by Dokyung</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dokyung is driving and Haeyoung1 is meditating</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Haeyoung1 is meditating</t>
-  </si>
-  <si>
-    <t>Dokyung calls Haeyoung1 by text and Haeyoung1 goes to the front of the house.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dokyung and Haeyoung1 talk about when they first saw each other, and Dokyung confides his situation to Haeyoung1.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Deogi tells Haeyoung1 to ask Dokyung to come in for breakfast.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dokyung waits leaning against the car in front of Haeyoung1’s house.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Deogi, Kyungsu, Haeyoung1, and Dokyung eat breakfast together</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Taejin looks at shoes of Taejin's partner while driving and notices that Taejin's partner was at the Chairman's house.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Haeyoung1 hugs Dokyung and kisses him.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dokyung sits in a recording studio and sings with his eyes closed.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17회</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -845,12 +911,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1134,8 +1203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1145,317 +1214,328 @@
     <col min="3" max="3" width="26.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55.125" customWidth="1"/>
     <col min="5" max="5" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>113</v>
+      <c r="A1" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" t="s">
         <v>168</v>
       </c>
-      <c r="D2" t="s">
-        <v>170</v>
-      </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D12" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C14" t="s">
         <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C15" t="s">
         <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C16" t="s">
         <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C17" t="s">
         <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C19" t="s">
         <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1463,16 +1543,16 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1480,16 +1560,16 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C21" t="s">
         <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1497,16 +1577,16 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C22" t="s">
         <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1514,16 +1594,16 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C23" t="s">
         <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1531,16 +1611,16 @@
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C24" t="s">
         <v>32</v>
       </c>
       <c r="D24" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E24" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1548,16 +1628,16 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C25" t="s">
         <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1565,16 +1645,16 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C26" t="s">
         <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1582,16 +1662,16 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C27" t="s">
         <v>35</v>
       </c>
       <c r="D27" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1599,16 +1679,16 @@
         <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C28" t="s">
         <v>36</v>
       </c>
       <c r="D28" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1616,16 +1696,16 @@
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C29" t="s">
         <v>37</v>
       </c>
       <c r="D29" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1633,16 +1713,16 @@
         <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C30" t="s">
         <v>38</v>
       </c>
       <c r="D30" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1650,16 +1730,16 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C31" t="s">
         <v>39</v>
       </c>
       <c r="D31" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1667,33 +1747,33 @@
         <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C32" t="s">
         <v>40</v>
       </c>
       <c r="D32" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E32" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B33" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C33" t="s">
         <v>41</v>
       </c>
       <c r="D33" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1701,33 +1781,33 @@
         <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C34" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D34" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E34" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B35" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C35" t="s">
         <v>42</v>
       </c>
       <c r="D35" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E35" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1735,33 +1815,33 @@
         <v>14</v>
       </c>
       <c r="B36" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C36" t="s">
         <v>43</v>
       </c>
       <c r="D36" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E36" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B37" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C37" t="s">
         <v>44</v>
       </c>
       <c r="D37" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E37" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1769,10 +1849,10 @@
         <v>45</v>
       </c>
       <c r="D38" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E38" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1780,10 +1860,10 @@
         <v>46</v>
       </c>
       <c r="D39" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E39" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1791,10 +1871,10 @@
         <v>47</v>
       </c>
       <c r="D40" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E40" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1802,10 +1882,10 @@
         <v>48</v>
       </c>
       <c r="D41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1813,10 +1893,10 @@
         <v>49</v>
       </c>
       <c r="D42" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E42" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1824,10 +1904,10 @@
         <v>50</v>
       </c>
       <c r="D43" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E43" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1835,10 +1915,10 @@
         <v>51</v>
       </c>
       <c r="D44" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1846,84 +1926,123 @@
         <v>52</v>
       </c>
       <c r="D45" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E45" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
         <v>53</v>
       </c>
+      <c r="D46" t="s">
+        <v>219</v>
+      </c>
       <c r="E46" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C47" t="s">
         <v>54</v>
       </c>
+      <c r="D47" t="s">
+        <v>220</v>
+      </c>
       <c r="E47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
         <v>55</v>
       </c>
+      <c r="D48" t="s">
+        <v>221</v>
+      </c>
       <c r="E48" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C49" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D49" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C50" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D50" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D51" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D52" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D53" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D54" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D55" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C56" t="s">
+        <v>229</v>
+      </c>
+      <c r="D56" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>231</v>
+      </c>
+      <c r="D57" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C57" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C58" t="s">
-        <v>65</v>
+      <c r="D58" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>